<commit_message>
update the readme file
update the readme file and added an overview page for the coal plant xlsx
</commit_message>
<xml_diff>
--- a/Asset Data/IGP/Asset_Data_IGP/Coal Plants/Coal_Plants_IGP/Coal_Plants_IGP_28_01_25 .xlsx
+++ b/Asset Data/IGP/Asset_Data_IGP/Coal Plants/Coal_Plants_IGP/Coal_Plants_IGP_28_01_25 .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ERASMUS\France_Sem3\side projects\APAD_oxford\Final_Dataset_Folder\APAD-Asset-Data\Asset Data\IGP\Asset_Data_IGP\Coal Plants\Coal_Plants_IGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6DDB6AD2-B462-4DCB-83F9-0BD3318270EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D82D98-68AF-4549-A3D0-C95895C3B20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C3C8C26B-282A-4DDC-88E2-67912F7BC31C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C3C8C26B-282A-4DDC-88E2-67912F7BC31C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="236">
   <si>
     <t>plant_name</t>
   </si>
@@ -656,9 +656,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>Project Name</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -668,296 +665,77 @@
     <t>Contact Person</t>
   </si>
   <si>
-    <t xml:space="preserve">Hassan Sheikh (Email: hassan.sheikh@smithschool.ox.ac.uk) </t>
-  </si>
-  <si>
-    <t>Contact Email</t>
-  </si>
-  <si>
-    <t>apad.world.proj@gmail.com</t>
-  </si>
-  <si>
     <t>Column Name</t>
   </si>
   <si>
-    <r>
-      <t>plant_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Name of the power plant.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>country</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Country where the plant is located.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>cap_all</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Combined capacity for all units (in MW).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>total_cap</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Total capacity of the plant (in MW).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>sts_all</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Status of all plant units.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>units</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Number of units in the power plant.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Operational status of the plant (e.g., active, inactive, planned).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>prod_kw</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Total electricity produced (in kilowatts).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>nox_ef</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Nitrogen oxide emission factor (tons per MW).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>nox_tn_y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Total nitrogen oxide emissions (in tons per year).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>so2_ef</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Sulfur dioxide emission factor (tons per MW).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>so2_tn_y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Total sulfur dioxide emissions (in tons per year).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>p10_ef</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Particulate matter (PM10) emission factor (tons per MW).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>p10_tn_y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Total PM10 emissions (in tons per year).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pm25_ef</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Particulate matter (PM2.5) emission factor (tons per MW).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>p25_tn_y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Total PM2.5 emissions (in tons per year).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>lat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Latitude of the plant’s location.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>lon</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Longitude of the plant’s location.</t>
-    </r>
-  </si>
-  <si>
-    <t>Coal Plants IGP</t>
+    <t>The Coal Plant dataset is a comprehensive collection of data detailing various aspects of coal power plants for the Indo-Gangetic Plain (IGP) region spanning Pakistan, India, and Bangladesh. This dataset includes information on plant locations, capacities, emissions, operational status, and other relevant attributes. The primary goal of this dataset is to enable the monitoring and analysis of air pollution and its impact on the environment and public health.</t>
+  </si>
+  <si>
+    <t>https://github.com/APAD2024/APAD-Asset-Data/tree/main/Asset%20Data/IGP/Asset_Data_IGP/Coal%20Plants/Coal_Plants_IGP</t>
+  </si>
+  <si>
+    <t>Hassan Sheikh (Email: hassan.sheikh@smithschool.ox.ac.uk) OR apad.world.proj@gmail.com</t>
+  </si>
+  <si>
+    <t>Name of the power plant.</t>
+  </si>
+  <si>
+    <t>Country where the plant is located.</t>
+  </si>
+  <si>
+    <t>Total capacity for all the plant units (in MW).</t>
+  </si>
+  <si>
+    <t>Status of all plant units.</t>
+  </si>
+  <si>
+    <t>Number of units for the power plant.</t>
+  </si>
+  <si>
+    <t>Annual electricity production (in kWh).</t>
+  </si>
+  <si>
+    <t>Current overall status of the plant (operating, permitted, etc.).</t>
+  </si>
+  <si>
+    <t>List of generation capacities (in MW) of each unit within the plant.</t>
+  </si>
+  <si>
+    <t>Total nitrogen oxide emissions (in tons per year).</t>
+  </si>
+  <si>
+    <t>Nitrogen oxide emission factor (grams per kWh [g/kWh]).</t>
+  </si>
+  <si>
+    <t>Sulfur dioxide emission factor (grams per kWh [g/kWh]).</t>
+  </si>
+  <si>
+    <t>Total sulfur dioxide emissions (in tons per year).</t>
+  </si>
+  <si>
+    <t>Particulate matter (PM10) emission factor (grams per kWh [g/kWh]).</t>
+  </si>
+  <si>
+    <t>Total PM10 emissions (in tons per year).</t>
+  </si>
+  <si>
+    <t>Particulate matter (PM2.5) emission factor (grams per kWh [g/kWh]).</t>
+  </si>
+  <si>
+    <t>Total PM2.5 emissions (in tons per year).</t>
+  </si>
+  <si>
+    <t>Latitude of the plant’s location.</t>
+  </si>
+  <si>
+    <t>Longitude of the plant’s location.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1107,8 +885,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F2328"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1288,6 +1072,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1465,20 +1255,25 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1855,247 +1650,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359CDFF6-7FBD-4793-9522-A22E617388D8}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="155.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="39" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" ht="28.8" customHeight="1">
       <c r="A4" t="s">
         <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>212</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>213</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" t="s">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>216</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>217</v>
+      <c r="B9" s="2" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>220</v>
+        <v>2</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>221</v>
+        <v>3</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>222</v>
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2103,7 +1892,7 @@
     <mergeCell ref="A1:O2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{9D8591A8-2B07-4646-B1C6-4F314F11E5D1}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{05884D7F-4168-4AC0-9BC9-82E230E709D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2113,65 +1902,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF18A7F-11FD-4FA1-A071-CCB4BC971080}">
   <dimension ref="A1:R111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="6" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:18" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>